<commit_message>
Post merge. Lidt problemer med CET
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/techdata_main_catalog.xlsx
+++ b/examples/Abatement/Data/techdata_main_catalog.xlsx
@@ -439,7 +439,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G4" sqref="G4"/>
+      <selection pane="topRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +549,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G3" sqref="G3"/>
+      <selection pane="topRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>